<commit_message>
fix import pemasukan pengeluaran covering
</commit_message>
<xml_diff>
--- a/public/template/FORMAT_IMPORT_STOK BAHAN_BAKU_COVERING.xlsx
+++ b/public/template/FORMAT_IMPORT_STOK BAHAN_BAKU_COVERING.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19635" windowHeight="7620"/>
+    <workbookView windowWidth="20490" windowHeight="7860" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PEMASUKAN" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>TEMPLATE DATA STOK BAHAN BAKU UNTUK PEMASUKAN COVERING</t>
   </si>
@@ -60,13 +60,13 @@
     <t>NOTE :</t>
   </si>
   <si>
-    <t>70D/24F</t>
+    <t>70D/20F</t>
   </si>
   <si>
     <t>NYLON</t>
   </si>
   <si>
-    <t>Black</t>
+    <t>BLACK</t>
   </si>
   <si>
     <t>NIM XIAMEN</t>
@@ -78,15 +78,6 @@
     <t>JIKA PEMASUKAN ANGKA POSITIF</t>
   </si>
   <si>
-    <t>70D/24N</t>
-  </si>
-  <si>
-    <t>White</t>
-  </si>
-  <si>
-    <t>XIAMEN</t>
-  </si>
-  <si>
     <t>JIKA PENGELUARAN ANGKA NEGATIF</t>
   </si>
   <si>
@@ -97,12 +88,6 @@
   </si>
   <si>
     <t>Anti Y</t>
-  </si>
-  <si>
-    <t>40D/12N</t>
-  </si>
-  <si>
-    <t>Anti X</t>
   </si>
 </sst>
 </file>
@@ -110,13 +95,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="5">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="yyyy\-mm\-yy"/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="180" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,6 +141,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF67748E"/>
+      <name val="Open Sans"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
@@ -301,7 +292,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,6 +314,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -707,67 +704,64 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -779,77 +773,80 @@
     <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -868,7 +865,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -892,28 +889,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1451,8 +1457,8 @@
   <sheetPr/>
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4"/>
@@ -1493,9 +1499,9 @@
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="9"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
     </row>
     <row r="3" ht="15.75" spans="1:12">
       <c r="A3" s="10" t="s">
@@ -1520,15 +1526,15 @@
         <v>8</v>
       </c>
       <c r="H3" s="4"/>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="18"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="21"/>
     </row>
     <row r="4" ht="15.75" spans="1:12">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="11" t="s">
@@ -1540,50 +1546,34 @@
       <c r="D4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="12">
-        <v>5</v>
-      </c>
+      <c r="E4" s="12"/>
       <c r="F4" s="11">
         <v>10</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="21"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="24"/>
     </row>
     <row r="5" ht="15.75" spans="1:12">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="13"/>
+      <c r="I5" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="12">
-        <v>5</v>
-      </c>
-      <c r="F5" s="11">
-        <v>10</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="21"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1600,13 +1590,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.2857142857143" customWidth="1"/>
     <col min="2" max="2" width="16.4285714285714" customWidth="1"/>
@@ -1645,7 +1635,7 @@
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="9"/>
-      <c r="I2" s="14"/>
+      <c r="I2" s="18"/>
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
     </row>
@@ -1672,7 +1662,7 @@
         <v>8</v>
       </c>
       <c r="H3" s="4"/>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="19" t="s">
         <v>9</v>
       </c>
       <c r="J3" s="4"/>
@@ -1680,55 +1670,67 @@
     </row>
     <row r="4" ht="15.75" spans="1:9">
       <c r="A4" s="11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="12">
-        <v>10</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E4" s="12"/>
       <c r="F4" s="11">
-        <v>-20</v>
+        <v>-2</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="19" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="1:9">
-      <c r="A5" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="12">
-        <v>10</v>
-      </c>
-      <c r="F5" s="11">
-        <v>-20</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>19</v>
-      </c>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="13"/>
+      <c r="I5" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="5:6">
+      <c r="E8" s="14"/>
+      <c r="F8" s="15"/>
+    </row>
+    <row r="9" spans="5:6">
+      <c r="E9" s="14"/>
+      <c r="F9" s="15"/>
+    </row>
+    <row r="10" spans="5:6">
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+    </row>
+    <row r="11" spans="5:6">
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+    </row>
+    <row r="12" spans="5:6">
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+    </row>
+    <row r="13" spans="5:6">
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+    </row>
+    <row r="14" spans="5:6">
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>